<commit_message>
Edited toothrow AB term
</commit_message>
<xml_diff>
--- a/terms/teethTerms.xlsx
+++ b/terms/teethTerms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Documents\GitHub\fovt\terms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA705BB-9D8D-4FB4-865A-B910FB534817}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F72C3D-90CC-471E-9A41-FAFF020264DF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" firstSheet="6" activeTab="9" xr2:uid="{02AD6335-DCEB-E448-89DC-D4459AEF2DA1}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11596" firstSheet="6" activeTab="10" xr2:uid="{02AD6335-DCEB-E448-89DC-D4459AEF2DA1}"/>
   </bookViews>
   <sheets>
     <sheet name="molars" sheetId="1" r:id="rId1"/>
@@ -4890,7 +4890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E1BF5A-9D40-754F-98C1-3B489ED02366}">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -5259,8 +5259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05D49CD-491C-4440-858F-42EEE0666E89}">
   <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -5576,7 +5576,7 @@
         <v>571</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>1150</v>
+        <v>1152</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>1151</v>
@@ -5587,7 +5587,7 @@
         <v>572</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>1153</v>

</xml_diff>